<commit_message>
fix some bugs in readme
</commit_message>
<xml_diff>
--- a/purchase_list.xlsx
+++ b/purchase_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\开源网课\github_ws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52725A51-E5E2-4AEB-92F3-229C908F7404}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310BD62C-BE6F-4A75-BF7D-2432C5BDA972}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1839,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB2B767-2823-4771-915E-E7BC0035A5D0}">
   <dimension ref="B3:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2249,7 +2249,7 @@
         <v>580</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:H25" si="2">F23*G23</f>
+        <f t="shared" ref="H23:H24" si="2">F23*G23</f>
         <v>580</v>
       </c>
       <c r="I23" t="s">

</xml_diff>